<commit_message>
fix TTD buffer bug ivtnmr.xls
</commit_message>
<xml_diff>
--- a/sample_prep/ivtnmr.xlsx
+++ b/sample_prep/ivtnmr.xlsx
@@ -81,12 +81,6 @@
     <t>TotalVolume</t>
   </si>
   <si>
-    <t>Plasmd~30nM final</t>
-  </si>
-  <si>
-    <t>20x TTD pH 7.7</t>
-  </si>
-  <si>
     <t>Often-modified variables</t>
   </si>
   <si>
@@ -106,6 +100,12 @@
   </si>
   <si>
     <t>T7 RNA Pol - put into eppendorf on ice. Add after recording time0 references</t>
+  </si>
+  <si>
+    <t>20x TTD pH 7.7 (minus protein volume)</t>
+  </si>
+  <si>
+    <t>Final: Plasmd~30nM or Oligo~1uM.</t>
   </si>
 </sst>
 </file>
@@ -815,7 +815,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -869,10 +869,10 @@
       <c r="H4" s="4"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:14" s="2" customFormat="1">
+    <row r="5" spans="1:14" s="2" customFormat="1" ht="40">
       <c r="A5" s="25"/>
       <c r="B5" s="24" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C5" s="28">
         <v>0.33</v>
@@ -894,13 +894,13 @@
       <c r="H5" s="7"/>
       <c r="I5" s="3" t="str">
         <f t="shared" ref="I5:I11" si="1">B5</f>
-        <v>Plasmd~30nM final</v>
+        <v>Final: Plasmd~30nM or Oligo~1uM.</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="2" customFormat="1">
       <c r="A6" s="1"/>
       <c r="B6" s="6" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1">
         <v>20</v>
@@ -916,13 +916,13 @@
         <v>20</v>
       </c>
       <c r="G6" s="5">
-        <f>TotalVolume/F6</f>
-        <v>22.5</v>
+        <f>(TotalVolume-ProteinVolume)/F6</f>
+        <v>20.8125</v>
       </c>
       <c r="H6" s="22"/>
       <c r="I6" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>20x TTD pH 7.7</v>
+        <v>20x TTD pH 7.7 (minus protein volume)</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1">
@@ -1041,7 +1041,7 @@
     <row r="11" spans="1:14" s="2" customFormat="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="20"/>
@@ -1114,7 +1114,7 @@
     <row r="15" spans="1:14" s="2" customFormat="1" ht="24" thickBot="1">
       <c r="A15" s="1"/>
       <c r="B15" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" s="32">
         <v>2000</v>
@@ -1153,7 +1153,7 @@
     <row r="17" spans="1:10" s="2" customFormat="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="9"/>
@@ -1174,7 +1174,7 @@
     <row r="18" spans="1:10" s="2" customFormat="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1232,7 +1232,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="5">
         <f>$C$2-SUM(G5:G19)</f>
-        <v>196.64999999999998</v>
+        <v>198.33749999999998</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="3" t="str">
@@ -1242,17 +1242,17 @@
     </row>
     <row r="25" spans="1:10" ht="23">
       <c r="B25" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="23">
       <c r="B26" s="31" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="B28" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>